<commit_message>
CAV Export still needs to be fixed for rows
</commit_message>
<xml_diff>
--- a/Table 4a Schedules/AHU 1_Table4a.xlsx
+++ b/Table 4a Schedules/AHU 1_Table4a.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rush\OneDrive - SC Engineers\Documents\Desktop\PsychroCalc\Table 4a Schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rushikesh/Documents/PsychroCalc/Table 4a Schedules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA62DF4D-E4CC-47FE-A857-2D8CE4F95E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E6540AA-D1F9-4345-9297-479CA47E90F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2E7656F7-CEC7-40C2-A08E-5D379BEC02DC}"/>
+    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{70F17B98-1B1A-C94C-AFB6-6C94965BE9D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="22">
   <si>
     <t>ROOM</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>PATIENT ROOM</t>
-  </si>
-  <si>
-    <t>NO REQUIREMENT FOR CONTINUOUS DIRECTIONAL CONTROL</t>
   </si>
 </sst>
 </file>
@@ -116,7 +113,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -636,27 +633,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A44A7D56-E7C1-406E-A145-ACBEBEE80B33}" name="AHU 1Table4A" displayName="AHU_1Table4A" ref="A1:R13" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:R13" xr:uid="{A44A7D56-E7C1-406E-A145-ACBEBEE80B33}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14A57F70-4E16-DC48-83A3-27C32F8D249B}" name="AHU 1Table4A" displayName="AHU_1Table4A" ref="A1:R13" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:R13" xr:uid="{14A57F70-4E16-DC48-83A3-27C32F8D249B}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{6D646F6C-1320-4AC9-85FF-36810F4C03ED}" name="ROOM" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{694F636B-44D0-426A-B310-D3DBD376C409}" name="ROOM #" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{2B1E50B4-601E-4350-9DDC-B1E38A3A537B}" name="AREA (FT²)" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{3A269908-28C6-4AD5-9D90-09FDB5DEB4B8}" name="HG_x000a_(FT)" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{6F78EAF9-5789-4F80-97E7-81E9DCFEB6BC}" name="TOTAL AC/HR" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{E03C3B5D-5BD3-4BDB-AEBC-DB23B6BE5EF7}" name="100%_x000a_EA" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{1176A426-9AC8-4E8A-BD18-0866E41CAA6B}" name="EA_x000a_(CFM)" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{B84B6F43-AC93-44EC-928A-AD017BB05291}" name="LOAD CFM" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{4F10F861-446E-4278-8939-AB68AAAC0A03}" name="AC/HR CFM" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{17CD88BD-EA14-4B82-B732-B68B6A287BB2}" name="4-A DESIGNATION" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{50176180-4CF7-4981-9A8B-9951A1CC1F79}" name="AIRBALANCE RELATIONSHIP" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{BDA65872-D722-4330-9638-42DC86642A2B}" name="MINIMUM OSA CHANGES PER HOUR" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{862677E9-8EAD-482E-8BC7-951ACACEF763}" name="OSA CFM" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{3B6B5265-3601-4E03-A46F-22C7E02965E6}" name="ALL AIR EXHAUSTED" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{42DE7884-B1A5-46B6-8EA1-152B1CAE08BD}" name="CALCULATED SA CFM" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{63C59A59-BD40-4B09-9E97-ABDD0F8EB48C}" name="DESIGN SA CFM" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{99BBB504-D7F6-4C45-B127-028117C864F4}" name="RA CFM" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{400727A0-BABC-4A86-B206-D073D37BD6EF}" name="EA CFM" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B6485D51-6152-C441-8871-0DF9A7885F79}" name="ROOM" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{211FE045-BE0B-774A-A48B-D6FD4BFED3E0}" name="ROOM #" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{D141E51C-D5A9-E040-9512-E6F68B98D4E0}" name="AREA (FT²)" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{FE140630-2A3A-DE4B-912F-1909D29E1B8B}" name="HG_x000a_(FT)" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{2A02F429-A7BB-0F42-BCCC-80D9A67F0329}" name="TOTAL AC/HR" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{A4812ACC-93BC-FE4F-98D7-F6294E2334DB}" name="100%_x000a_EA" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{942B14AA-9ECC-7B43-B896-BDB652D38F31}" name="EA_x000a_(CFM)" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{325D2980-8CBF-7246-8773-D81A0CD7B101}" name="LOAD CFM" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{F03EB34C-47F1-914D-AADB-B0FAA1E8C00F}" name="AC/HR CFM" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{8B3DE8E3-1E7C-8F40-AA14-9CC7AA3A1D45}" name="4-A DESIGNATION" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{4E0CEEB4-BBAB-B74D-9911-21C2297E015A}" name="AIRBALANCE RELATIONSHIP" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{ED354AA7-FC68-C745-8A74-3A3A77E36A2E}" name="MINIMUM OSA CHANGES PER HOUR" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{90F664AB-F431-6943-9F29-A105BD2B3617}" name="OSA CFM" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{974C251D-E2C6-4B42-9059-D284B627B3FA}" name="ALL AIR EXHAUSTED" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{C09FD1AD-D976-C442-B884-DB2A350B355D}" name="CALCULATED SA CFM" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{D35545DA-850F-044F-B00E-7AC155C6685D}" name="DESIGN SA CFM" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{D7460AC1-2BC8-4A46-8605-7C6C77B872DC}" name="RA CFM" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{84B5D789-C733-3649-ADEE-E6D471DFD7DA}" name="EA CFM" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -958,36 +955,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87BD971-46B1-4070-B0ED-A984D48F9370}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27C6791-E8A6-9849-ADC0-720E1F2AE286}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="70.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1075,7 +1073,7 @@
         <v>21</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L2" s="1">
         <v>2</v>
@@ -1099,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1131,7 +1129,7 @@
         <v>21</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L3" s="1">
         <v>2</v>
@@ -1155,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1187,7 +1185,7 @@
         <v>21</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L4" s="1">
         <v>2</v>
@@ -1211,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1243,7 +1241,7 @@
         <v>21</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L5" s="1">
         <v>2</v>
@@ -1267,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1299,7 +1297,7 @@
         <v>21</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L6" s="1">
         <v>2</v>
@@ -1323,7 +1321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1355,7 +1353,7 @@
         <v>21</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L7" s="1">
         <v>2</v>
@@ -1379,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1411,7 +1409,7 @@
         <v>21</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L8" s="1">
         <v>2</v>
@@ -1435,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1467,7 +1465,7 @@
         <v>21</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L9" s="1">
         <v>2</v>
@@ -1491,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1523,7 +1521,7 @@
         <v>21</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L10" s="1">
         <v>2</v>
@@ -1547,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1579,7 +1577,7 @@
         <v>21</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L11" s="1">
         <v>2</v>
@@ -1603,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1635,7 +1633,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L12" s="1">
         <v>2</v>
@@ -1659,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1">

</xml_diff>